<commit_message>
wbs 수정, properties 수정
</commit_message>
<xml_diff>
--- a/doc/bizmap/비즈맵 개발 wbs.xlsx
+++ b/doc/bizmap/비즈맵 개발 wbs.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="81">
   <si>
     <t>depth 1</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -98,10 +98,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>분석페이지</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>기본보고서</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -235,18 +231,6 @@
   </si>
   <si>
     <t>/bizmap/subscribe</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/flowpop</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/bizmap/flowpop/getFlowpop</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/density</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -346,6 +330,26 @@
   </si>
   <si>
     <t>/youTube</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/flowpop</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/bizmap/flowpop/getFlowpop</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/density</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/rising</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/bizmap/rising/getRisingUpjong</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -767,10 +771,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I38"/>
+  <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -800,35 +804,35 @@
         <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G1" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="H1" s="3" t="s">
-        <v>46</v>
-      </c>
       <c r="I1" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
@@ -854,7 +858,7 @@
         <v>5</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
@@ -869,7 +873,7 @@
         <v>6</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -884,7 +888,7 @@
         <v>7</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
@@ -899,7 +903,7 @@
         <v>8</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
@@ -914,7 +918,7 @@
         <v>9</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
@@ -929,10 +933,14 @@
         <v>10</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
+        <v>35</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>55</v>
+      </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
@@ -957,16 +965,16 @@
         <v>12</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
@@ -976,13 +984,13 @@
         <v>14</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
@@ -995,18 +1003,18 @@
         <v>13</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="2" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
@@ -1016,7 +1024,7 @@
         <v>15</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
@@ -1031,7 +1039,7 @@
         <v>17</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
@@ -1046,23 +1054,23 @@
         <v>16</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="7"/>
+      <c r="B17" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="4"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
@@ -1073,35 +1081,43 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="7"/>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="4"/>
+      <c r="C18" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
+      <c r="D18" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" ht="33" x14ac:dyDescent="0.3">
       <c r="A19" s="7"/>
       <c r="B19" s="4"/>
       <c r="C19" s="1" t="s">
         <v>20</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
+      <c r="I19" s="2" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="20" spans="1:9" ht="33" x14ac:dyDescent="0.3">
       <c r="A20" s="7"/>
@@ -1110,39 +1126,39 @@
         <v>21</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
       <c r="I20" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="33" x14ac:dyDescent="0.3">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="7"/>
       <c r="B21" s="4"/>
       <c r="C21" s="1" t="s">
         <v>22</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
       <c r="I21" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
@@ -1152,48 +1168,46 @@
         <v>23</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
-      <c r="I22" s="2" t="s">
-        <v>77</v>
-      </c>
+      <c r="I22" s="1"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="7"/>
-      <c r="B23" s="4"/>
-      <c r="C23" s="1" t="s">
+      <c r="B23" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D23" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>47</v>
-      </c>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="7"/>
-      <c r="B24" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>48</v>
+      </c>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
@@ -1202,220 +1216,216 @@
       <c r="A25" s="7"/>
       <c r="B25" s="4"/>
       <c r="C25" s="1" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>63</v>
+        <v>76</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>49</v>
+        <v>77</v>
       </c>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
-      <c r="I25" s="1"/>
+      <c r="I25" s="1" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="7"/>
-      <c r="B26" s="4"/>
-      <c r="C26" s="1" t="s">
+      <c r="B26" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D26" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>54</v>
-      </c>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
-      <c r="I26" s="1" t="s">
-        <v>68</v>
-      </c>
+      <c r="I26" s="1"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="7"/>
-      <c r="B27" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
+      <c r="B27" s="4"/>
+      <c r="C27" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>48</v>
+      </c>
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
-      <c r="I27" s="1"/>
+      <c r="I27" s="1" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="7"/>
       <c r="B28" s="4"/>
       <c r="C28" s="1" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
       <c r="I28" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="7"/>
       <c r="B29" s="4"/>
       <c r="C29" s="1" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>63</v>
+        <v>78</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
       <c r="I29" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="7"/>
-      <c r="B30" s="4"/>
-      <c r="C30" s="1" t="s">
+      <c r="B30" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D30" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>56</v>
-      </c>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
-      <c r="I30" s="1" t="s">
-        <v>71</v>
-      </c>
+      <c r="I30" s="1"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="7"/>
-      <c r="B31" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
-      <c r="F31" s="1"/>
+      <c r="B31" s="4"/>
+      <c r="C31" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>48</v>
+      </c>
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
-      <c r="I31" s="1"/>
+      <c r="I31" s="1" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="7"/>
       <c r="B32" s="4"/>
       <c r="C32" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>63</v>
+        <v>79</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>49</v>
+        <v>80</v>
       </c>
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
-      <c r="I32" s="1" t="s">
-        <v>69</v>
+      <c r="I32" s="2" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" s="7"/>
       <c r="B33" s="4"/>
       <c r="C33" s="1" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
-      <c r="I33" s="2" t="s">
-        <v>72</v>
-      </c>
+      <c r="I33" s="1"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="7"/>
-      <c r="B34" s="4"/>
-      <c r="C34" s="1" t="s">
+      <c r="B34" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D34" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>58</v>
-      </c>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A35" s="7"/>
-      <c r="B35" s="4" t="s">
+      <c r="A35" s="8"/>
+      <c r="B35" s="4"/>
+      <c r="C35" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
-      <c r="E35" s="1"/>
-      <c r="F35" s="1"/>
+      <c r="D35" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>74</v>
+      </c>
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A36" s="8"/>
+      <c r="A36" s="4" t="s">
+        <v>32</v>
+      </c>
       <c r="B36" s="4"/>
-      <c r="C36" s="1" t="s">
-        <v>32</v>
-      </c>
+      <c r="C36" s="1"/>
       <c r="D36" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E36" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>78</v>
-      </c>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
       <c r="G36" s="1"/>
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
@@ -1424,44 +1434,29 @@
       <c r="A37" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B37" s="4"/>
-      <c r="C37" s="1"/>
+      <c r="B37" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>42</v>
+      </c>
       <c r="D37" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E37" s="1"/>
-      <c r="F37" s="1"/>
+        <v>36</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>55</v>
+      </c>
       <c r="G37" s="1"/>
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A38" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B38" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="F38" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="G38" s="1"/>
-      <c r="H38" s="1"/>
-      <c r="I38" s="1"/>
-    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A2:A16"/>
-    <mergeCell ref="A17:A36"/>
+    <mergeCell ref="A17:A35"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>